<commit_message>
Fixed update bugs in inputDateTimeInline. Implemented month editor sortie row duration calculation and display.  Linked takeoff inputs to land inputs to fill in defaults.
</commit_message>
<xml_diff>
--- a/MsnLog Schema (005).xlsx
+++ b/MsnLog Schema (005).xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21231"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1375906852E\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\peter\OneDrive\Workspace\Hawk Log\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3E61539F-75F1-4738-9B10-4AEDE3E30DFE}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="210" windowWidth="28800" windowHeight="12225"/>
+    <workbookView xWindow="2685" yWindow="3660" windowWidth="28800" windowHeight="15435" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="388" uniqueCount="212">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1414" uniqueCount="215">
   <si>
     <t>Name</t>
   </si>
@@ -71,15 +72,9 @@
     <t>schedTakeoff</t>
   </si>
   <si>
-    <t>schedLanding</t>
-  </si>
-  <si>
     <t>actualTakeoff</t>
   </si>
   <si>
-    <t>actualLanding</t>
-  </si>
-  <si>
     <t>Date + Time</t>
   </si>
   <si>
@@ -122,9 +117,6 @@
     <t>COCOM</t>
   </si>
   <si>
-    <t>tailNum</t>
-  </si>
-  <si>
     <t>Aircraft:TailNum</t>
   </si>
   <si>
@@ -147,12 +139,6 @@
   </si>
   <si>
     <t>"11-2020","12-2045"</t>
-  </si>
-  <si>
-    <t>Effective</t>
-  </si>
-  <si>
-    <t>EffReason</t>
   </si>
   <si>
     <t>"Effective", "Ineffective", "Partially Effective", "WX Cancel", "MX RTB", "Ops Cancel"</t>
@@ -470,12 +456,6 @@
     <t>"Late entry due to delayed takeoff"</t>
   </si>
   <si>
-    <t>takeoffNote</t>
-  </si>
-  <si>
-    <t>landingNote</t>
-  </si>
-  <si>
     <t>"Late due to ATC traffic"</t>
   </si>
   <si>
@@ -733,12 +713,42 @@
   <si>
     <t>"11-2020","12-2045" **USE Timeline to track tail swap events - if we expand to cover Config Sheet info, will need another table for spares</t>
   </si>
+  <si>
+    <t>String (4 char)</t>
+  </si>
+  <si>
+    <t>KBAB</t>
+  </si>
+  <si>
+    <t>TakeoffAirfield</t>
+  </si>
+  <si>
+    <t>TakeoffNote</t>
+  </si>
+  <si>
+    <t>Reason</t>
+  </si>
+  <si>
+    <t>Naming conventions: CamelCase, NoSpace, StartWithCaps except sched/actual prefixes (unless that seems crazy, then just make those like the others)</t>
+  </si>
+  <si>
+    <t>LandAirfield</t>
+  </si>
+  <si>
+    <t>schedLand</t>
+  </si>
+  <si>
+    <t>actualLand</t>
+  </si>
+  <si>
+    <t>LandNote</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -772,6 +782,20 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFCC00FF"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF00B050"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="7"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -881,7 +905,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="52">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -994,6 +1018,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1317,12 +1343,12 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M169"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:M171"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <selection pane="bottomLeft" activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1347,7 +1373,7 @@
         <v>2</v>
       </c>
       <c r="J1" s="2" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -1359,7 +1385,7 @@
       <c r="D2" s="16"/>
       <c r="E2" s="4"/>
       <c r="J2" t="s">
-        <v>111</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -1370,7 +1396,7 @@
         <v>5</v>
       </c>
       <c r="J3" t="s">
-        <v>112</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="30" x14ac:dyDescent="0.25">
@@ -1384,7 +1410,7 @@
         <v>11</v>
       </c>
       <c r="J4" t="s">
-        <v>113</v>
+        <v>108</v>
       </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
@@ -1397,275 +1423,275 @@
       <c r="D5" s="15" t="s">
         <v>10</v>
       </c>
+      <c r="J5" t="s">
+        <v>210</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="C6" s="1" t="s">
-        <v>28</v>
-      </c>
       <c r="D6" s="15" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>14</v>
+      <c r="B7" s="52" t="s">
+        <v>207</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>19</v>
+        <v>206</v>
       </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>15</v>
+      <c r="B8" s="52" t="s">
+        <v>211</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>205</v>
       </c>
       <c r="D8" s="15" t="s">
-        <v>20</v>
+        <v>206</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="C9" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B10" s="53" t="s">
+        <v>212</v>
+      </c>
+      <c r="C10" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D10" s="15" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B11" s="48" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="D9" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>16</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D10" s="15" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>17</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D11" s="15" t="s">
-        <v>21</v>
       </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
-        <v>24</v>
+        <v>15</v>
       </c>
       <c r="C12" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B13" s="53" t="s">
+        <v>213</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="B14" s="48" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="D12" s="15" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>144</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D13" s="15" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="B14" t="s">
-        <v>145</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>28</v>
-      </c>
-      <c r="D14" s="15" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
-        <v>30</v>
+        <v>208</v>
       </c>
       <c r="C15" s="1" t="s">
-        <v>38</v>
+        <v>26</v>
       </c>
       <c r="D15" s="15" t="s">
-        <v>36</v>
+        <v>10</v>
       </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
-        <v>31</v>
+        <v>214</v>
       </c>
       <c r="C16" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="D16" s="15" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B17" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="D16" s="15" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+      <c r="D17" s="15" t="s">
         <v>33</v>
-      </c>
-      <c r="B17" t="s">
-        <v>32</v>
-      </c>
-      <c r="C17" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>211</v>
       </c>
     </row>
     <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B18" t="s">
+        <v>29</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" s="15" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" t="s">
+        <v>44</v>
+      </c>
+      <c r="C19" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D19" s="15" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B20" s="53" t="s">
+        <v>48</v>
+      </c>
+      <c r="C20" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="D20" s="15" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B21" s="53" t="s">
+        <v>209</v>
+      </c>
+      <c r="C21" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="C18" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="D18" s="15" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B19" t="s">
+      <c r="D21" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A23" s="5" t="s">
         <v>42</v>
       </c>
-      <c r="C19" s="1" t="s">
-        <v>46</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B21" s="6"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="17"/>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="2" t="s">
-        <v>49</v>
-      </c>
-      <c r="C22" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B23" t="s">
-        <v>50</v>
-      </c>
-      <c r="C23" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>52</v>
-      </c>
+      <c r="B23" s="6"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="17"/>
     </row>
     <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>58</v>
-      </c>
-      <c r="B24" t="s">
-        <v>56</v>
+        <v>43</v>
+      </c>
+      <c r="B24" s="2" t="s">
+        <v>44</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D24" s="15" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
+        <v>45</v>
+      </c>
+      <c r="C25" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D25" s="15" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>53</v>
       </c>
-      <c r="C25" s="1" t="s">
+      <c r="B26" t="s">
+        <v>51</v>
+      </c>
+      <c r="C26" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D25" s="15" t="s">
+    </row>
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B27" t="s">
+        <v>48</v>
+      </c>
+      <c r="C27" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D27" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B28" t="s">
+        <v>24</v>
+      </c>
+      <c r="C28" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D28" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="26" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B26" t="s">
-        <v>26</v>
-      </c>
-      <c r="C26" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28" s="9"/>
-      <c r="C28" s="10"/>
-      <c r="D28" s="18"/>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>48</v>
-      </c>
-      <c r="B29" s="2" t="s">
-        <v>63</v>
-      </c>
-      <c r="C29" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D29" s="15" t="s">
-        <v>64</v>
-      </c>
-    </row>
     <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B30" t="s">
-        <v>65</v>
-      </c>
-      <c r="C30" s="1" t="s">
-        <v>37</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>66</v>
-      </c>
+      <c r="A30" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="B30" s="9"/>
+      <c r="C30" s="10"/>
+      <c r="D30" s="18"/>
     </row>
     <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
+        <v>43</v>
+      </c>
+      <c r="B31" s="2" t="s">
         <v>58</v>
       </c>
-      <c r="B31" t="s">
-        <v>56</v>
-      </c>
       <c r="C31" s="1" t="s">
-        <v>57</v>
+        <v>31</v>
       </c>
       <c r="D31" s="15" t="s">
         <v>59</v>
@@ -1673,1188 +1699,1213 @@
     </row>
     <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
+        <v>60</v>
+      </c>
+      <c r="C32" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="D32" s="15" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="1" t="s">
+      <c r="B33" t="s">
+        <v>51</v>
+      </c>
+      <c r="C33" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="D33" s="15" t="s">
         <v>54</v>
       </c>
-      <c r="D32" s="15" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="33" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B33" t="s">
-        <v>26</v>
-      </c>
-      <c r="C33" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D33" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A35" s="33" t="s">
-        <v>210</v>
-      </c>
-      <c r="B35" s="33" t="s">
-        <v>209</v>
-      </c>
-      <c r="C35" s="34"/>
-      <c r="D35" s="35"/>
-    </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+    </row>
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B34" t="s">
         <v>48</v>
       </c>
-      <c r="B36" s="2" t="s">
+      <c r="C34" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="D34" s="15" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B35" t="s">
+        <v>24</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D35" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A37" s="33" t="s">
+        <v>203</v>
+      </c>
+      <c r="B37" s="33" t="s">
+        <v>202</v>
+      </c>
+      <c r="C37" s="34"/>
+      <c r="D37" s="35"/>
+    </row>
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
+        <v>43</v>
+      </c>
+      <c r="B38" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A37" s="1" t="s">
-        <v>90</v>
-      </c>
-      <c r="B37" t="s">
-        <v>208</v>
-      </c>
-      <c r="C37" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D37" s="15" t="s">
+    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A39" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="B39" t="s">
+        <v>201</v>
+      </c>
+      <c r="C39" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D39" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A40" s="1"/>
+      <c r="B40" t="s">
+        <v>167</v>
+      </c>
+      <c r="C40" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D40" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A41" s="1"/>
+      <c r="B41" t="s">
+        <v>168</v>
+      </c>
+      <c r="C41" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="D41" s="15" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="B42" t="s">
+        <v>24</v>
+      </c>
+      <c r="C42" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" s="15" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A44" s="13" t="s">
+        <v>63</v>
+      </c>
+      <c r="B44" s="13" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A38" s="1"/>
-      <c r="B38" t="s">
-        <v>174</v>
-      </c>
-      <c r="C38" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D38" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A39" s="1"/>
-      <c r="B39" t="s">
-        <v>175</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>78</v>
-      </c>
-      <c r="D39" s="15" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="40" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="B40" t="s">
-        <v>26</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>61</v>
-      </c>
-      <c r="D40" s="15" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
-        <v>68</v>
-      </c>
-      <c r="B42" s="13" t="s">
-        <v>69</v>
-      </c>
-      <c r="C42" s="14"/>
-      <c r="D42" s="19"/>
-    </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
-        <v>48</v>
-      </c>
-      <c r="B43" s="2" t="s">
-        <v>5</v>
-      </c>
-      <c r="D43" s="15" t="s">
-        <v>122</v>
-      </c>
-    </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
-        <v>133</v>
-      </c>
-      <c r="B44" t="s">
-        <v>114</v>
-      </c>
-      <c r="D44" s="15" t="s">
-        <v>115</v>
-      </c>
+      <c r="C44" s="14"/>
+      <c r="D44" s="19"/>
     </row>
     <row r="45" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>72</v>
-      </c>
-      <c r="B45" t="s">
-        <v>70</v>
-      </c>
-      <c r="C45" s="1" t="s">
-        <v>37</v>
+        <v>43</v>
+      </c>
+      <c r="B45" s="2" t="s">
+        <v>5</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>71</v>
+        <v>117</v>
       </c>
     </row>
     <row r="46" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A46" t="s">
+        <v>128</v>
+      </c>
       <c r="B46" t="s">
-        <v>190</v>
-      </c>
-      <c r="C46" s="1" t="s">
-        <v>191</v>
+        <v>109</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>192</v>
+        <v>110</v>
       </c>
     </row>
     <row r="47" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A47" t="s">
+        <v>67</v>
+      </c>
       <c r="B47" t="s">
-        <v>0</v>
+        <v>65</v>
       </c>
       <c r="C47" s="1" t="s">
-        <v>79</v>
+        <v>34</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>80</v>
+        <v>66</v>
       </c>
     </row>
     <row r="48" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="C48" s="1" t="s">
-        <v>51</v>
+        <v>184</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>81</v>
+        <v>185</v>
       </c>
     </row>
     <row r="49" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>0</v>
+      </c>
+      <c r="C49" s="1" t="s">
         <v>74</v>
       </c>
-      <c r="C49" s="1" t="s">
-        <v>78</v>
+      <c r="D49" s="15" t="s">
+        <v>75</v>
       </c>
     </row>
     <row r="50" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B50" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
       <c r="C50" s="1" t="s">
-        <v>78</v>
+        <v>46</v>
+      </c>
+      <c r="D50" s="15" t="s">
+        <v>76</v>
       </c>
     </row>
     <row r="51" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B51" t="s">
-        <v>76</v>
+        <v>69</v>
       </c>
       <c r="C51" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
     </row>
     <row r="52" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B52" t="s">
-        <v>82</v>
+        <v>70</v>
       </c>
       <c r="C52" s="1" t="s">
-        <v>23</v>
+        <v>73</v>
       </c>
     </row>
     <row r="53" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B53" t="s">
-        <v>83</v>
+        <v>71</v>
       </c>
       <c r="C53" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
+      </c>
+      <c r="D53" s="15" t="s">
+        <v>72</v>
       </c>
     </row>
     <row r="54" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B54" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C54" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="55" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B55" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C55" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="56" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B56" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C56" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="57" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B57" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C57" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="58" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B58" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="C58" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="59" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A59" t="s">
-        <v>90</v>
-      </c>
       <c r="B59" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="15" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
     </row>
     <row r="60" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B60" t="s">
+        <v>83</v>
+      </c>
+      <c r="C60" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A61" t="s">
+        <v>85</v>
+      </c>
+      <c r="B61" t="s">
+        <v>84</v>
+      </c>
+      <c r="C61" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="D61" s="15" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="62" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>86</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="D62" s="15" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="63" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="64" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="C64" s="1" t="s">
         <v>91</v>
       </c>
-      <c r="C60" s="1" t="s">
+    </row>
+    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A66" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="B66" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D60" s="15" t="s">
+      <c r="C66" s="12"/>
+      <c r="D66" s="20"/>
+    </row>
+    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A67" t="s">
+        <v>43</v>
+      </c>
+      <c r="B67" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A68" t="s">
+        <v>128</v>
+      </c>
+      <c r="B68" t="s">
+        <v>109</v>
+      </c>
+      <c r="D68" s="15" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="69" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B69" t="s">
         <v>93</v>
       </c>
-    </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B61" t="s">
+      <c r="C69" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="D69" s="15" t="s">
         <v>94</v>
-      </c>
-    </row>
-    <row r="62" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="C62" s="1" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A64" s="11" t="s">
-        <v>95</v>
-      </c>
-      <c r="B64" s="11" t="s">
-        <v>97</v>
-      </c>
-      <c r="C64" s="12"/>
-      <c r="D64" s="20"/>
-    </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A65" t="s">
-        <v>48</v>
-      </c>
-      <c r="B65" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A66" t="s">
-        <v>133</v>
-      </c>
-      <c r="B66" t="s">
-        <v>114</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B67" t="s">
-        <v>98</v>
-      </c>
-      <c r="C67" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B68" t="s">
-        <v>65</v>
-      </c>
-      <c r="C68" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D68" s="15" t="s">
-        <v>100</v>
-      </c>
-    </row>
-    <row r="69" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A69" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B69" t="s">
-        <v>101</v>
-      </c>
-      <c r="C69" s="1" t="s">
-        <v>102</v>
-      </c>
-      <c r="D69" s="15" t="s">
-        <v>103</v>
       </c>
     </row>
     <row r="70" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B70" t="s">
-        <v>0</v>
+        <v>60</v>
       </c>
       <c r="C70" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>104</v>
-      </c>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.25">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="71" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A71" s="1" t="s">
+        <v>100</v>
+      </c>
       <c r="B71" t="s">
-        <v>106</v>
+        <v>96</v>
       </c>
       <c r="C71" s="1" t="s">
-        <v>79</v>
+        <v>97</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
     </row>
     <row r="72" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B72" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="C72" s="1" t="s">
-        <v>27</v>
+        <v>74</v>
+      </c>
+      <c r="D72" s="15" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="73" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B73" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C73" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D73" s="15" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="74" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>24</v>
+      </c>
+      <c r="C74" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>103</v>
+      </c>
+      <c r="C75" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="D75" s="15">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>118</v>
+      </c>
+      <c r="B77" s="24"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="26"/>
+    </row>
+    <row r="78" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A78" t="s">
+        <v>43</v>
+      </c>
+      <c r="B78" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A79" t="s">
+        <v>128</v>
+      </c>
+      <c r="B79" t="s">
         <v>109</v>
       </c>
-      <c r="D73" s="15">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A75" s="24" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="24"/>
-      <c r="C75" s="25"/>
-      <c r="D75" s="26"/>
-    </row>
-    <row r="76" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A76" t="s">
-        <v>48</v>
-      </c>
-      <c r="B76" s="2" t="s">
+      <c r="D79" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="80" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A80" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B80" t="s">
+        <v>113</v>
+      </c>
+      <c r="C80" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D80" s="15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>121</v>
+      </c>
+      <c r="C81" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="D81" s="15" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>24</v>
+      </c>
+      <c r="C82" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D82" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A84" s="27" t="s">
+        <v>119</v>
+      </c>
+      <c r="B84" s="27" t="s">
+        <v>122</v>
+      </c>
+      <c r="C84" s="28"/>
+      <c r="D84" s="29"/>
+    </row>
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A85" t="s">
+        <v>43</v>
+      </c>
+      <c r="B85" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="77" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A77" t="s">
-        <v>133</v>
-      </c>
-      <c r="B77" t="s">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A86" t="s">
+        <v>128</v>
+      </c>
+      <c r="B86" t="s">
+        <v>109</v>
+      </c>
+      <c r="D86" s="15" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="87" spans="1:4" ht="30" x14ac:dyDescent="0.25">
+      <c r="A87" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B87" t="s">
+        <v>127</v>
+      </c>
+      <c r="C87" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D87" s="15" t="s">
         <v>114</v>
-      </c>
-      <c r="D77" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="78" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A78" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B78" t="s">
-        <v>118</v>
-      </c>
-      <c r="C78" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D78" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="79" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B79" t="s">
-        <v>126</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D79" s="15" t="s">
-        <v>130</v>
-      </c>
-    </row>
-    <row r="80" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B80" t="s">
-        <v>26</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>120</v>
-      </c>
-      <c r="D80" s="15" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A82" s="27" t="s">
-        <v>124</v>
-      </c>
-      <c r="B82" s="27" t="s">
-        <v>127</v>
-      </c>
-      <c r="C82" s="28"/>
-      <c r="D82" s="29"/>
-    </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A83" t="s">
-        <v>48</v>
-      </c>
-      <c r="B83" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A84" t="s">
-        <v>133</v>
-      </c>
-      <c r="B84" t="s">
-        <v>114</v>
-      </c>
-      <c r="D84" s="15" t="s">
-        <v>117</v>
-      </c>
-    </row>
-    <row r="85" spans="1:4" ht="30" x14ac:dyDescent="0.25">
-      <c r="A85" s="1" t="s">
-        <v>105</v>
-      </c>
-      <c r="B85" t="s">
-        <v>132</v>
-      </c>
-      <c r="C85" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D85" s="15" t="s">
-        <v>119</v>
-      </c>
-    </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B86" t="s">
-        <v>131</v>
-      </c>
-      <c r="C86" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D86" s="15" t="s">
-        <v>128</v>
-      </c>
-    </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B87" t="s">
-        <v>126</v>
-      </c>
-      <c r="C87" s="1" t="s">
-        <v>125</v>
-      </c>
-      <c r="D87" s="15" t="s">
-        <v>129</v>
       </c>
     </row>
     <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B88" t="s">
-        <v>26</v>
+        <v>126</v>
       </c>
       <c r="C88" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D88" s="15" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>121</v>
+      </c>
+      <c r="C89" s="1" t="s">
         <v>120</v>
       </c>
-      <c r="D88" s="15" t="s">
-        <v>121</v>
+      <c r="D89" s="15" t="s">
+        <v>124</v>
       </c>
     </row>
     <row r="90" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A90" s="30" t="s">
-        <v>134</v>
-      </c>
-      <c r="B90" s="30"/>
-      <c r="C90" s="31"/>
-      <c r="D90" s="32"/>
-    </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A91" t="s">
-        <v>48</v>
-      </c>
-      <c r="B91" s="2" t="s">
+      <c r="B90" t="s">
+        <v>24</v>
+      </c>
+      <c r="C90" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="D90" s="15" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A92" s="30" t="s">
+        <v>129</v>
+      </c>
+      <c r="B92" s="30"/>
+      <c r="C92" s="31"/>
+      <c r="D92" s="32"/>
+    </row>
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A93" t="s">
+        <v>43</v>
+      </c>
+      <c r="B93" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A92" t="s">
-        <v>133</v>
-      </c>
-      <c r="B92" t="s">
-        <v>114</v>
-      </c>
-      <c r="D92" s="15" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B93" t="s">
-        <v>0</v>
-      </c>
-      <c r="C93" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="D93" s="15" t="s">
-        <v>136</v>
-      </c>
-    </row>
     <row r="94" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A94" t="s">
+        <v>128</v>
+      </c>
       <c r="B94" t="s">
-        <v>138</v>
-      </c>
-      <c r="C94" s="1" t="s">
-        <v>18</v>
+        <v>109</v>
       </c>
       <c r="D94" s="15" t="s">
-        <v>142</v>
+        <v>130</v>
       </c>
     </row>
     <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B95" t="s">
-        <v>139</v>
+        <v>0</v>
       </c>
       <c r="C95" s="1" t="s">
-        <v>18</v>
+        <v>132</v>
       </c>
       <c r="D95" s="15" t="s">
-        <v>142</v>
+        <v>131</v>
       </c>
     </row>
     <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B96" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C96" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D96" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B97" t="s">
-        <v>141</v>
+        <v>134</v>
       </c>
       <c r="C97" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D97" s="15" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
     </row>
     <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B98" t="s">
-        <v>22</v>
+        <v>135</v>
       </c>
       <c r="C98" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D98" s="15" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
     </row>
     <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B99" t="s">
-        <v>24</v>
+        <v>136</v>
       </c>
       <c r="C99" s="1" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
       <c r="D99" s="15" t="s">
-        <v>25</v>
+        <v>137</v>
       </c>
     </row>
     <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B100" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="C100" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="D100" s="15" t="s">
-        <v>143</v>
+        <v>23</v>
+      </c>
+    </row>
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B101" t="s">
+        <v>22</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D101" s="15" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="102" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A102" s="45" t="s">
-        <v>193</v>
-      </c>
-      <c r="B102" s="45" t="s">
-        <v>189</v>
-      </c>
-      <c r="C102" s="46"/>
-      <c r="D102" s="47"/>
-    </row>
-    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A103" t="s">
-        <v>48</v>
-      </c>
-      <c r="B103" s="2" t="s">
-        <v>70</v>
-      </c>
-      <c r="C103" s="1" t="s">
-        <v>37</v>
+      <c r="B102" t="s">
+        <v>24</v>
+      </c>
+      <c r="C102" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D102" s="15" t="s">
+        <v>138</v>
       </c>
     </row>
     <row r="104" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B104" t="s">
-        <v>190</v>
-      </c>
-      <c r="C104" s="1" t="s">
-        <v>191</v>
-      </c>
-      <c r="D104" s="15" t="s">
-        <v>192</v>
-      </c>
+      <c r="A104" s="45" t="s">
+        <v>186</v>
+      </c>
+      <c r="B104" s="45" t="s">
+        <v>182</v>
+      </c>
+      <c r="C104" s="46"/>
+      <c r="D104" s="47"/>
     </row>
     <row r="105" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B105" t="s">
-        <v>0</v>
+      <c r="A105" t="s">
+        <v>43</v>
+      </c>
+      <c r="B105" s="2" t="s">
+        <v>65</v>
       </c>
       <c r="C105" s="1" t="s">
-        <v>79</v>
-      </c>
-      <c r="D105" s="15" t="s">
-        <v>80</v>
+        <v>34</v>
       </c>
     </row>
     <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B106" t="s">
-        <v>73</v>
+        <v>183</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>51</v>
+        <v>184</v>
       </c>
       <c r="D106" s="15" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A109" s="49" t="s">
-        <v>172</v>
-      </c>
-      <c r="B109" s="49"/>
-      <c r="C109" s="50"/>
-      <c r="D109" s="51"/>
-      <c r="E109" s="49"/>
-      <c r="F109" s="49"/>
-      <c r="G109" s="49"/>
-      <c r="H109" s="49"/>
-      <c r="I109" s="49"/>
-      <c r="J109" s="49"/>
-      <c r="K109" s="49"/>
-      <c r="L109" s="49"/>
-      <c r="M109" s="49"/>
+        <v>185</v>
+      </c>
+    </row>
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>0</v>
+      </c>
+      <c r="C107" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D107" s="15" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>68</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="D108" s="15" t="s">
+        <v>76</v>
+      </c>
     </row>
     <row r="111" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A111" s="39" t="s">
+      <c r="A111" s="49" t="s">
         <v>165</v>
       </c>
-      <c r="B111" s="39"/>
-      <c r="C111" s="40" t="s">
-        <v>164</v>
-      </c>
-      <c r="D111" s="41"/>
-    </row>
-    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="A112" t="s">
-        <v>48</v>
-      </c>
-      <c r="B112" s="2" t="s">
+      <c r="B111" s="49"/>
+      <c r="C111" s="50"/>
+      <c r="D111" s="51"/>
+      <c r="E111" s="49"/>
+      <c r="F111" s="49"/>
+      <c r="G111" s="49"/>
+      <c r="H111" s="49"/>
+      <c r="I111" s="49"/>
+      <c r="J111" s="49"/>
+      <c r="K111" s="49"/>
+      <c r="L111" s="49"/>
+      <c r="M111" s="49"/>
+    </row>
+    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A113" s="39" t="s">
+        <v>158</v>
+      </c>
+      <c r="B113" s="39"/>
+      <c r="C113" s="40" t="s">
+        <v>157</v>
+      </c>
+      <c r="D113" s="41"/>
+    </row>
+    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A114" t="s">
+        <v>43</v>
+      </c>
+      <c r="B114" s="2" t="s">
         <v>5</v>
-      </c>
-    </row>
-    <row r="113" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A113" t="s">
-        <v>161</v>
-      </c>
-      <c r="B113" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="114" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B114" t="s">
-        <v>170</v>
       </c>
     </row>
     <row r="115" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A115" t="s">
-        <v>171</v>
+        <v>154</v>
       </c>
       <c r="B115" t="s">
-        <v>169</v>
+        <v>160</v>
+      </c>
+    </row>
+    <row r="116" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>163</v>
       </c>
     </row>
     <row r="117" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A117" s="21" t="s">
-        <v>147</v>
-      </c>
-      <c r="B117" s="21"/>
-      <c r="C117" s="22"/>
-      <c r="D117" s="23"/>
-    </row>
-    <row r="118" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A118" t="s">
-        <v>48</v>
-      </c>
-      <c r="B118" s="2" t="s">
+      <c r="A117" t="s">
+        <v>164</v>
+      </c>
+      <c r="B117" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A119" s="21" t="s">
+        <v>140</v>
+      </c>
+      <c r="B119" s="21"/>
+      <c r="C119" s="22"/>
+      <c r="D119" s="23"/>
+    </row>
+    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A120" t="s">
+        <v>43</v>
+      </c>
+      <c r="B120" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="119" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A119" t="s">
-        <v>161</v>
-      </c>
-      <c r="B119" t="s">
-        <v>162</v>
-      </c>
-      <c r="D119" s="15" t="s">
-        <v>163</v>
-      </c>
-    </row>
-    <row r="120" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B120" t="s">
-        <v>148</v>
-      </c>
-      <c r="C120" s="1" t="s">
-        <v>153</v>
-      </c>
-    </row>
     <row r="121" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A121" t="s">
+        <v>154</v>
+      </c>
       <c r="B121" t="s">
-        <v>149</v>
-      </c>
-      <c r="C121" s="1" t="s">
-        <v>109</v>
+        <v>155</v>
+      </c>
+      <c r="D121" s="15" t="s">
+        <v>156</v>
       </c>
     </row>
     <row r="122" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B122" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="C122" s="1" t="s">
-        <v>109</v>
+        <v>146</v>
       </c>
     </row>
     <row r="123" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B123" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C123" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="124" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B124" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="C124" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="125" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B125" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C125" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="126" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B126" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="C126" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="127" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B127" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="C127" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="128" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B128" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C128" s="1" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="129" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B129" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
       <c r="C129" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D129" s="15" t="s">
-        <v>204</v>
+        <v>104</v>
       </c>
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B130" t="s">
-        <v>158</v>
+        <v>150</v>
       </c>
       <c r="C130" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D130" s="15" t="s">
-        <v>205</v>
+        <v>104</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B131" t="s">
-        <v>203</v>
+        <v>152</v>
       </c>
       <c r="C131" s="1" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="D131" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
+      </c>
+    </row>
+    <row r="132" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>151</v>
+      </c>
+      <c r="C132" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D132" s="15" t="s">
+        <v>198</v>
       </c>
     </row>
     <row r="133" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A133" s="36" t="s">
+      <c r="B133" t="s">
+        <v>196</v>
+      </c>
+      <c r="C133" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D133" s="15" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A135" s="36" t="s">
+        <v>159</v>
+      </c>
+      <c r="B135" s="36" t="s">
+        <v>153</v>
+      </c>
+      <c r="C135" s="37"/>
+      <c r="D135" s="38"/>
+    </row>
+    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B136" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A137" t="s">
+        <v>190</v>
+      </c>
+      <c r="B137" t="s">
+        <v>161</v>
+      </c>
+      <c r="D137" s="15" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="138" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>187</v>
+      </c>
+      <c r="C138" s="1" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>188</v>
+      </c>
+      <c r="C139" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="D139" s="15" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A141" s="30" t="s">
         <v>166</v>
       </c>
-      <c r="B133" s="36" t="s">
-        <v>160</v>
-      </c>
-      <c r="C133" s="37"/>
-      <c r="D133" s="38"/>
-    </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B134" s="2" t="s">
+      <c r="B141" s="30"/>
+      <c r="C141" s="31"/>
+      <c r="D141" s="32"/>
+    </row>
+    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B142" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A135" t="s">
-        <v>197</v>
-      </c>
-      <c r="B135" t="s">
-        <v>168</v>
-      </c>
-      <c r="D135" s="15" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B136" t="s">
-        <v>194</v>
-      </c>
-      <c r="C136" s="1" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B137" t="s">
-        <v>195</v>
-      </c>
-      <c r="C137" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D137" s="15" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A139" s="30" t="s">
-        <v>173</v>
-      </c>
-      <c r="B139" s="30"/>
-      <c r="C139" s="31"/>
-      <c r="D139" s="32"/>
-    </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B140" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A141" t="s">
-        <v>161</v>
-      </c>
-      <c r="B141" t="s">
-        <v>162</v>
-      </c>
-      <c r="D141" s="15" t="s">
-        <v>183</v>
-      </c>
-    </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B142" t="s">
-        <v>174</v>
-      </c>
-      <c r="C142" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
     <row r="143" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A143" t="s">
+        <v>154</v>
+      </c>
       <c r="B143" t="s">
-        <v>175</v>
-      </c>
-      <c r="C143" s="1" t="s">
-        <v>18</v>
+        <v>155</v>
+      </c>
+      <c r="D143" s="15" t="s">
+        <v>176</v>
       </c>
     </row>
     <row r="144" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B144" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C144" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="145" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B145" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C145" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="146" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B146" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
       <c r="C146" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D146" s="15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="147" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B147" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="C147" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D147" s="15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="148" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B148" t="s">
-        <v>199</v>
+        <v>20</v>
       </c>
       <c r="C148" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D148" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="D148" s="15" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="149" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B149" t="s">
-        <v>201</v>
+        <v>22</v>
       </c>
       <c r="C149" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D149" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="D149" s="15" t="s">
-        <v>207</v>
       </c>
     </row>
     <row r="150" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B150" t="s">
-        <v>178</v>
+        <v>192</v>
+      </c>
+      <c r="C150" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D150" s="15" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="151" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B151" t="s">
-        <v>179</v>
+        <v>194</v>
+      </c>
+      <c r="C151" s="1" t="s">
+        <v>21</v>
       </c>
       <c r="D151" s="15" t="s">
-        <v>182</v>
+        <v>200</v>
       </c>
     </row>
     <row r="152" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B152" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
     </row>
     <row r="153" spans="1:4" x14ac:dyDescent="0.25">
       <c r="B153" t="s">
-        <v>26</v>
-      </c>
-      <c r="C153" s="1" t="s">
-        <v>27</v>
+        <v>172</v>
       </c>
       <c r="D153" s="15" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="156" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A156" s="42" t="s">
-        <v>184</v>
-      </c>
-      <c r="B156" s="42"/>
-      <c r="C156" s="43"/>
-      <c r="D156" s="44"/>
-    </row>
-    <row r="157" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B157" s="2" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="154" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B154" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="155" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B155" t="s">
+        <v>24</v>
+      </c>
+      <c r="C155" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="D155" s="15" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A158" s="42" t="s">
+        <v>177</v>
+      </c>
+      <c r="B158" s="42"/>
+      <c r="C158" s="43"/>
+      <c r="D158" s="44"/>
+    </row>
+    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B159" s="2" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="158" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A158" t="s">
-        <v>161</v>
-      </c>
-      <c r="B158" t="s">
-        <v>162</v>
-      </c>
-      <c r="D158" s="15" t="s">
-        <v>185</v>
-      </c>
-    </row>
-    <row r="159" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="B159" t="s">
-        <v>186</v>
-      </c>
-      <c r="C159" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="D159" s="15" t="s">
-        <v>187</v>
-      </c>
-    </row>
     <row r="160" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A160" t="s">
+        <v>154</v>
+      </c>
       <c r="B160" t="s">
-        <v>174</v>
-      </c>
-      <c r="C160" s="1" t="s">
-        <v>18</v>
+        <v>155</v>
+      </c>
+      <c r="D160" s="15" t="s">
+        <v>178</v>
       </c>
     </row>
     <row r="161" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B161" t="s">
-        <v>175</v>
+        <v>179</v>
       </c>
       <c r="C161" s="1" t="s">
-        <v>18</v>
+        <v>8</v>
+      </c>
+      <c r="D161" s="15" t="s">
+        <v>180</v>
       </c>
     </row>
     <row r="162" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B162" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="C162" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="163" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B163" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C163" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
     </row>
     <row r="164" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B164" t="s">
-        <v>22</v>
+        <v>169</v>
       </c>
       <c r="C164" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D164" s="15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="165" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B165" t="s">
-        <v>24</v>
+        <v>170</v>
       </c>
       <c r="C165" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="D165" s="15" t="s">
-        <v>25</v>
+        <v>16</v>
       </c>
     </row>
     <row r="166" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B166" t="s">
-        <v>199</v>
+        <v>20</v>
       </c>
       <c r="C166" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D166" s="15" t="s">
         <v>23</v>
-      </c>
-      <c r="D166" s="15" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="167" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B167" t="s">
-        <v>201</v>
+        <v>22</v>
       </c>
       <c r="C167" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D167" s="15" t="s">
         <v>23</v>
       </c>
-      <c r="D167" s="15" t="s">
-        <v>202</v>
-      </c>
     </row>
     <row r="168" spans="2:4" x14ac:dyDescent="0.25">
-      <c r="B168" s="48" t="s">
-        <v>188</v>
+      <c r="B168" t="s">
+        <v>192</v>
+      </c>
+      <c r="C168" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="D168" s="15" t="s">
+        <v>193</v>
       </c>
     </row>
     <row r="169" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B169" t="s">
-        <v>26</v>
+        <v>194</v>
       </c>
       <c r="C169" s="1" t="s">
-        <v>27</v>
+        <v>21</v>
+      </c>
+      <c r="D169" s="15" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="170" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B170" s="48" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="171" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="B171" t="s">
+        <v>24</v>
+      </c>
+      <c r="C171" s="1" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>